<commit_message>
Wave effect added to the Vertex Shader
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EED9B0E-2DDE-4EF8-A483-EF398E50FC43}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC50F2C-3A2C-4B32-89A2-EC8106C783CD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="113">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -229,9 +229,6 @@
   </si>
   <si>
     <t>Simultaneous Loading of Textures or Models done with Multithreading &amp; D3DCreation Calls. (Win32 projects only)</t>
-  </si>
-  <si>
-    <t>Demonstrate modified vertex grid based on input map or sine wave in vertex shader. (ex: Waving Flag, Heightmap Terrain)</t>
   </si>
   <si>
     <t>Realtime scene reflections based on dynamic cube map rendertargets</t>
@@ -371,6 +368,18 @@
   </si>
   <si>
     <t>X</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>II</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Demonstrate modified vertex grid based on input map or sine wave in vertex shader. (ex: Waving Flag, Heightmap Terrain)</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -972,25 +981,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="106.5" customWidth="1"/>
-    <col min="2" max="2" width="25.5" customWidth="1"/>
+    <col min="1" max="1" width="106.44140625" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="7" width="25.5" customWidth="1"/>
-    <col min="8" max="9" width="25.875" customWidth="1"/>
-    <col min="10" max="11" width="24.5" customWidth="1"/>
-    <col min="12" max="12" width="24.125" customWidth="1"/>
-    <col min="13" max="14" width="9.125" customWidth="1"/>
+    <col min="4" max="7" width="25.44140625" customWidth="1"/>
+    <col min="8" max="9" width="25.88671875" customWidth="1"/>
+    <col min="10" max="11" width="24.44140625" customWidth="1"/>
+    <col min="12" max="12" width="24.109375" customWidth="1"/>
+    <col min="13" max="14" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1004,9 +1013,9 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -1042,7 +1051,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
@@ -1069,12 +1078,12 @@
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="5">
         <v>4</v>
@@ -1086,10 +1095,10 @@
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G4" s="16">
         <f t="shared" ref="G4:G67" si="0" xml:space="preserve"> IF(EXACT(F4,"X"),IF(EXACT(E4,"I"),$B4,IF(EXACT(E4,"II"),$C4,IF(EXACT(E4,"III"),$D4,0))),0)</f>
@@ -1109,16 +1118,16 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" s="5">
         <v>4</v>
@@ -1130,10 +1139,10 @@
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G5" s="16">
         <f t="shared" si="0"/>
@@ -1150,12 +1159,12 @@
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="5">
         <v>4</v>
@@ -1167,10 +1176,10 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="G6" s="16">
         <f t="shared" si="0"/>
@@ -1182,7 +1191,7 @@
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 20,0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J6" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) - 20,0)</f>
@@ -1194,9 +1203,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -1208,10 +1217,10 @@
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G7" s="16">
         <f t="shared" si="0"/>
@@ -1229,7 +1238,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>36</v>
       </c>
@@ -1243,10 +1252,10 @@
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G8" s="16">
         <f t="shared" si="0"/>
@@ -1262,12 +1271,12 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>37</v>
       </c>
@@ -1281,10 +1290,10 @@
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G9" s="16">
         <f t="shared" si="0"/>
@@ -1302,7 +1311,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>38</v>
       </c>
@@ -1316,10 +1325,10 @@
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G10" s="16">
         <f t="shared" si="0"/>
@@ -1327,11 +1336,11 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
@@ -1340,7 +1349,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>46</v>
       </c>
@@ -1365,7 +1374,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>53</v>
       </c>
@@ -1390,9 +1399,9 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -1415,9 +1424,9 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" s="5">
         <v>4</v>
@@ -1440,7 +1449,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>42</v>
       </c>
@@ -1465,7 +1474,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1482,7 +1491,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>48</v>
       </c>
@@ -1501,7 +1510,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1518,7 +1527,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1535,7 +1544,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>9</v>
       </c>
@@ -1554,9 +1563,9 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" s="5">
         <v>4</v>
@@ -1568,10 +1577,10 @@
         <v>2</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G21" s="16">
         <f t="shared" si="0"/>
@@ -1583,7 +1592,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>47</v>
       </c>
@@ -1608,9 +1617,9 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" s="5">
         <v>4</v>
@@ -1633,7 +1642,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>35</v>
       </c>
@@ -1647,10 +1656,10 @@
         <v>3</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G24" s="16">
         <f t="shared" si="0"/>
@@ -1662,9 +1671,9 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B25" s="5">
         <v>2</v>
@@ -1687,7 +1696,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1704,9 +1713,9 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1723,9 +1732,9 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B28" s="5">
         <v>3</v>
@@ -1737,10 +1746,10 @@
         <v>1</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="G28" s="16">
         <f t="shared" si="0"/>
@@ -1752,7 +1761,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>61</v>
       </c>
@@ -1777,7 +1786,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>63</v>
       </c>
@@ -1802,7 +1811,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>62</v>
       </c>
@@ -1827,7 +1836,7 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>64</v>
       </c>
@@ -1852,7 +1861,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>65</v>
       </c>
@@ -1877,7 +1886,7 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1894,7 +1903,7 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1911,7 +1920,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>49</v>
       </c>
@@ -1930,9 +1939,9 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B37" s="5">
         <v>3</v>
@@ -1944,10 +1953,10 @@
         <v>1</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G37" s="16">
         <f t="shared" si="0"/>
@@ -1959,9 +1968,9 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B38" s="5">
         <v>2</v>
@@ -1984,9 +1993,9 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B39" s="5">
         <v>4</v>
@@ -1998,10 +2007,10 @@
         <v>4</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G39" s="16">
         <f t="shared" si="0"/>
@@ -2013,9 +2022,9 @@
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B40" s="5">
         <v>4</v>
@@ -2038,7 +2047,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>41</v>
       </c>
@@ -2063,7 +2072,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>32</v>
       </c>
@@ -2088,7 +2097,7 @@
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>33</v>
       </c>
@@ -2113,7 +2122,7 @@
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>50</v>
       </c>
@@ -2138,7 +2147,7 @@
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>34</v>
       </c>
@@ -2163,9 +2172,9 @@
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
-        <v>67</v>
+        <v>112</v>
       </c>
       <c r="B46" s="1">
         <v>3</v>
@@ -2177,10 +2186,10 @@
         <v>2</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G46" s="16">
         <f t="shared" si="0"/>
@@ -2192,7 +2201,7 @@
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2209,7 +2218,7 @@
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2226,7 +2235,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>7</v>
       </c>
@@ -2245,9 +2254,9 @@
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B50" s="5">
         <v>3</v>
@@ -2270,7 +2279,7 @@
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>43</v>
       </c>
@@ -2295,7 +2304,7 @@
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>51</v>
       </c>
@@ -2320,9 +2329,9 @@
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B53" s="5">
         <v>4</v>
@@ -2345,7 +2354,7 @@
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2362,7 +2371,7 @@
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>6</v>
       </c>
@@ -2381,9 +2390,9 @@
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B56" s="5">
         <v>2</v>
@@ -2406,7 +2415,7 @@
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
         <v>60</v>
       </c>
@@ -2420,10 +2429,10 @@
         <v>2</v>
       </c>
       <c r="E57" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>110</v>
       </c>
       <c r="G57" s="16">
         <f t="shared" si="0"/>
@@ -2435,7 +2444,7 @@
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
         <v>66</v>
       </c>
@@ -2460,7 +2469,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>44</v>
       </c>
@@ -2485,7 +2494,7 @@
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2502,7 +2511,7 @@
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2519,7 +2528,7 @@
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>5</v>
       </c>
@@ -2538,9 +2547,9 @@
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B63" s="5">
         <v>2</v>
@@ -2551,11 +2560,15 @@
       <c r="D63" s="5">
         <v>2</v>
       </c>
-      <c r="E63" s="2"/>
-      <c r="F63" s="3"/>
+      <c r="E63" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>111</v>
+      </c>
       <c r="G63" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
@@ -2563,9 +2576,9 @@
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B64" s="5">
         <v>1</v>
@@ -2577,10 +2590,10 @@
         <v>1</v>
       </c>
       <c r="E64" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F64" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="G64" s="16">
         <f t="shared" si="0"/>
@@ -2592,9 +2605,9 @@
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B65" s="5">
         <v>1</v>
@@ -2617,7 +2630,7 @@
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
         <v>54</v>
       </c>
@@ -2631,10 +2644,10 @@
         <v>1</v>
       </c>
       <c r="E66" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F66" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="G66" s="16">
         <f t="shared" si="0"/>
@@ -2646,7 +2659,7 @@
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="21" t="s">
         <v>52</v>
       </c>
@@ -2660,10 +2673,10 @@
         <v>4</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G67" s="16">
         <f t="shared" si="0"/>
@@ -2675,7 +2688,7 @@
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
         <v>45</v>
       </c>
@@ -2700,7 +2713,7 @@
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2717,7 +2730,7 @@
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2734,7 +2747,7 @@
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>4</v>
       </c>
@@ -2753,9 +2766,9 @@
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B72" s="5">
         <v>2</v>
@@ -2778,9 +2791,9 @@
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B73" s="5">
         <v>1</v>
@@ -2803,9 +2816,9 @@
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B74" s="5">
         <v>2</v>
@@ -2828,9 +2841,9 @@
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B75" s="5">
         <v>3</v>
@@ -2853,9 +2866,9 @@
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B76" s="5">
         <v>2</v>
@@ -2878,9 +2891,9 @@
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B77" s="5">
         <v>3</v>
@@ -2903,9 +2916,9 @@
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B78" s="5">
         <v>3</v>
@@ -2928,7 +2941,7 @@
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="11"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
@@ -2945,7 +2958,7 @@
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="11"/>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
@@ -2962,9 +2975,9 @@
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
@@ -2981,7 +2994,7 @@
       <c r="K81" s="5"/>
       <c r="L81" s="5"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
         <v>58</v>
       </c>
@@ -3002,7 +3015,7 @@
       <c r="K82" s="5"/>
       <c r="L82" s="5"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
         <v>59</v>
       </c>
@@ -3023,9 +3036,9 @@
       <c r="K83" s="5"/>
       <c r="L83" s="5"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
@@ -3044,7 +3057,7 @@
       <c r="K84" s="5"/>
       <c r="L84" s="5"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
         <v>56</v>
       </c>
@@ -3065,7 +3078,7 @@
       <c r="K85" s="5"/>
       <c r="L85" s="5"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
         <v>55</v>
       </c>
@@ -3086,7 +3099,7 @@
       <c r="K86" s="5"/>
       <c r="L86" s="5"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
         <v>57</v>
       </c>
@@ -3107,7 +3120,7 @@
       <c r="K87" s="5"/>
       <c r="L87" s="5"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="8"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3124,7 +3137,7 @@
       <c r="K88" s="5"/>
       <c r="L88" s="5"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="8"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -3141,7 +3154,7 @@
       <c r="K89" s="5"/>
       <c r="L89" s="5"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>30</v>
       </c>
@@ -3165,7 +3178,7 @@
       <c r="K90" s="6"/>
       <c r="L90" s="5"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
         <v>17</v>
       </c>
@@ -3173,10 +3186,10 @@
         <v>2</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E91" s="3"/>
       <c r="F91" s="5"/>
@@ -3187,7 +3200,7 @@
       <c r="K91" s="6"/>
       <c r="L91" s="5"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
         <v>28</v>
       </c>
@@ -3195,10 +3208,10 @@
         <v>1</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E92" s="3"/>
       <c r="F92" s="5"/>
@@ -3209,7 +3222,7 @@
       <c r="K92" s="6"/>
       <c r="L92" s="5"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="11"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
@@ -3223,7 +3236,7 @@
       <c r="K93" s="6"/>
       <c r="L93" s="5"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="11"/>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
@@ -3237,78 +3250,78 @@
       <c r="K94" s="5"/>
       <c r="L94" s="5"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="12"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="12"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="12"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="12"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="12"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="12"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="12"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="12"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="12"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="12"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="12"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="12"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="12"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="12"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="12"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="12"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="12"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="12"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="12"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="12"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="12"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="13"/>
     </row>
   </sheetData>
@@ -3334,7 +3347,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3404,7 +3417,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3422,7 +3435,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Look at feature added
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC50F2C-3A2C-4B32-89A2-EC8106C783CD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34838DED-3BA6-45F5-B1AA-C8E483D61D85}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="115">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -380,6 +380,14 @@
   </si>
   <si>
     <t>Demonstrate modified vertex grid based on input map or sine wave in vertex shader. (ex: Waving Flag, Heightmap Terrain)</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>II</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -981,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1118,11 +1126,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1191,7 +1199,7 @@
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 20,0)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J6" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) - 20,0)</f>
@@ -1271,7 +1279,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1336,11 +1344,11 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
@@ -2618,11 +2626,15 @@
       <c r="D65" s="5">
         <v>1</v>
       </c>
-      <c r="E65" s="2"/>
-      <c r="F65" s="3"/>
+      <c r="E65" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="G65" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
@@ -3347,7 +3359,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Cleaned up some mess
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34838DED-3BA6-45F5-B1AA-C8E483D61D85}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1C5B3C-276D-4712-B5BE-412CA33782FA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="116">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -388,6 +388,10 @@
   </si>
   <si>
     <t>X</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>III</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -989,23 +993,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="106.44140625" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="1" max="1" width="106.5" customWidth="1"/>
+    <col min="2" max="2" width="25.5" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="7" width="25.44140625" customWidth="1"/>
-    <col min="8" max="9" width="25.88671875" customWidth="1"/>
-    <col min="10" max="11" width="24.44140625" customWidth="1"/>
-    <col min="12" max="12" width="24.109375" customWidth="1"/>
-    <col min="13" max="14" width="9.109375" customWidth="1"/>
+    <col min="4" max="7" width="25.5" customWidth="1"/>
+    <col min="8" max="9" width="25.875" customWidth="1"/>
+    <col min="10" max="11" width="24.5" customWidth="1"/>
+    <col min="12" max="12" width="24.125" customWidth="1"/>
+    <col min="13" max="14" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>102</v>
       </c>
@@ -1021,7 +1025,7 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
         <v>103</v>
       </c>
@@ -1059,7 +1063,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
@@ -1089,7 +1093,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
         <v>69</v>
       </c>
@@ -1133,7 +1137,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" s="10" t="s">
         <v>91</v>
       </c>
@@ -1170,7 +1174,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="10" t="s">
         <v>68</v>
       </c>
@@ -1211,7 +1215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="10" t="s">
         <v>95</v>
       </c>
@@ -1246,7 +1250,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8" s="20" t="s">
         <v>36</v>
       </c>
@@ -1284,7 +1288,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9" s="10" t="s">
         <v>37</v>
       </c>
@@ -1319,7 +1323,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10" s="20" t="s">
         <v>38</v>
       </c>
@@ -1357,7 +1361,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11" s="11" t="s">
         <v>46</v>
       </c>
@@ -1382,7 +1386,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" s="11" t="s">
         <v>53</v>
       </c>
@@ -1407,7 +1411,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" s="11" t="s">
         <v>73</v>
       </c>
@@ -1432,7 +1436,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A14" s="11" t="s">
         <v>74</v>
       </c>
@@ -1457,7 +1461,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15" s="10" t="s">
         <v>42</v>
       </c>
@@ -1470,7 +1474,9 @@
       <c r="D15" s="5">
         <v>2</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="16">
         <f t="shared" si="0"/>
@@ -1482,7 +1488,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16" s="11"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1499,7 +1505,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A17" s="8" t="s">
         <v>48</v>
       </c>
@@ -1518,7 +1524,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A18" s="11"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1535,7 +1541,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A19" s="8"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1552,7 +1558,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="s">
         <v>9</v>
       </c>
@@ -1571,7 +1577,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A21" s="10" t="s">
         <v>94</v>
       </c>
@@ -1600,7 +1606,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A22" s="11" t="s">
         <v>47</v>
       </c>
@@ -1625,7 +1631,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A23" s="20" t="s">
         <v>96</v>
       </c>
@@ -1650,7 +1656,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A24" s="10" t="s">
         <v>35</v>
       </c>
@@ -1679,7 +1685,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A25" s="20" t="s">
         <v>75</v>
       </c>
@@ -1704,7 +1710,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A26" s="8"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1721,7 +1727,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="s">
         <v>70</v>
       </c>
@@ -1740,7 +1746,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A28" s="10" t="s">
         <v>97</v>
       </c>
@@ -1769,7 +1775,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A29" s="11" t="s">
         <v>61</v>
       </c>
@@ -1794,7 +1800,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A30" s="10" t="s">
         <v>63</v>
       </c>
@@ -1819,7 +1825,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A31" s="11" t="s">
         <v>62</v>
       </c>
@@ -1844,7 +1850,7 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A32" s="11" t="s">
         <v>64</v>
       </c>
@@ -1869,7 +1875,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A33" s="11" t="s">
         <v>65</v>
       </c>
@@ -1894,7 +1900,7 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A34" s="8"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1911,7 +1917,7 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A35" s="8"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1928,7 +1934,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="s">
         <v>49</v>
       </c>
@@ -1947,7 +1953,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A37" s="20" t="s">
         <v>72</v>
       </c>
@@ -1976,7 +1982,7 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A38" s="10" t="s">
         <v>76</v>
       </c>
@@ -2001,7 +2007,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A39" s="10" t="s">
         <v>92</v>
       </c>
@@ -2030,7 +2036,7 @@
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A40" s="11" t="s">
         <v>90</v>
       </c>
@@ -2055,7 +2061,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A41" s="11" t="s">
         <v>41</v>
       </c>
@@ -2080,7 +2086,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A42" s="11" t="s">
         <v>32</v>
       </c>
@@ -2105,7 +2111,7 @@
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A43" s="11" t="s">
         <v>33</v>
       </c>
@@ -2130,7 +2136,7 @@
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A44" s="11" t="s">
         <v>50</v>
       </c>
@@ -2155,7 +2161,7 @@
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A45" s="11" t="s">
         <v>34</v>
       </c>
@@ -2180,7 +2186,7 @@
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A46" s="23" t="s">
         <v>112</v>
       </c>
@@ -2209,7 +2215,7 @@
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A47" s="22"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2226,7 +2232,7 @@
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A48" s="8"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2243,7 +2249,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A49" s="9" t="s">
         <v>7</v>
       </c>
@@ -2262,7 +2268,7 @@
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A50" s="11" t="s">
         <v>71</v>
       </c>
@@ -2287,7 +2293,7 @@
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A51" s="11" t="s">
         <v>43</v>
       </c>
@@ -2312,7 +2318,7 @@
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A52" s="11" t="s">
         <v>51</v>
       </c>
@@ -2337,7 +2343,7 @@
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A53" s="11" t="s">
         <v>67</v>
       </c>
@@ -2362,7 +2368,7 @@
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A54" s="8"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2379,7 +2385,7 @@
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A55" s="9" t="s">
         <v>6</v>
       </c>
@@ -2398,7 +2404,7 @@
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A56" s="11" t="s">
         <v>77</v>
       </c>
@@ -2423,7 +2429,7 @@
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A57" s="10" t="s">
         <v>60</v>
       </c>
@@ -2452,7 +2458,7 @@
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A58" s="11" t="s">
         <v>66</v>
       </c>
@@ -2477,7 +2483,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A59" s="11" t="s">
         <v>44</v>
       </c>
@@ -2502,7 +2508,7 @@
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A60" s="8"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2519,7 +2525,7 @@
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A61" s="8"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2536,7 +2542,7 @@
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A62" s="9" t="s">
         <v>5</v>
       </c>
@@ -2555,7 +2561,7 @@
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A63" s="10" t="s">
         <v>98</v>
       </c>
@@ -2584,7 +2590,7 @@
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A64" s="20" t="s">
         <v>93</v>
       </c>
@@ -2613,7 +2619,7 @@
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A65" s="20" t="s">
         <v>80</v>
       </c>
@@ -2642,7 +2648,7 @@
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A66" s="20" t="s">
         <v>54</v>
       </c>
@@ -2671,7 +2677,7 @@
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A67" s="21" t="s">
         <v>52</v>
       </c>
@@ -2700,7 +2706,7 @@
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A68" s="10" t="s">
         <v>45</v>
       </c>
@@ -2725,7 +2731,7 @@
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A69" s="8"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2742,7 +2748,7 @@
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A70" s="8"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2759,7 +2765,7 @@
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A71" s="9" t="s">
         <v>4</v>
       </c>
@@ -2778,7 +2784,7 @@
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A72" s="11" t="s">
         <v>83</v>
       </c>
@@ -2803,7 +2809,7 @@
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A73" s="11" t="s">
         <v>89</v>
       </c>
@@ -2828,7 +2834,7 @@
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A74" s="11" t="s">
         <v>84</v>
       </c>
@@ -2853,7 +2859,7 @@
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A75" s="11" t="s">
         <v>86</v>
       </c>
@@ -2878,7 +2884,7 @@
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A76" s="11" t="s">
         <v>85</v>
       </c>
@@ -2903,7 +2909,7 @@
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A77" s="11" t="s">
         <v>87</v>
       </c>
@@ -2928,7 +2934,7 @@
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A78" s="11" t="s">
         <v>88</v>
       </c>
@@ -2953,7 +2959,7 @@
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A79" s="11"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
@@ -2970,7 +2976,7 @@
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A80" s="11"/>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
@@ -2987,7 +2993,7 @@
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A81" s="9" t="s">
         <v>82</v>
       </c>
@@ -3006,7 +3012,7 @@
       <c r="K81" s="5"/>
       <c r="L81" s="5"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A82" s="11" t="s">
         <v>58</v>
       </c>
@@ -3027,7 +3033,7 @@
       <c r="K82" s="5"/>
       <c r="L82" s="5"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A83" s="11" t="s">
         <v>59</v>
       </c>
@@ -3048,7 +3054,7 @@
       <c r="K83" s="5"/>
       <c r="L83" s="5"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A84" s="11" t="s">
         <v>81</v>
       </c>
@@ -3069,7 +3075,7 @@
       <c r="K84" s="5"/>
       <c r="L84" s="5"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A85" s="11" t="s">
         <v>56</v>
       </c>
@@ -3090,7 +3096,7 @@
       <c r="K85" s="5"/>
       <c r="L85" s="5"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A86" s="11" t="s">
         <v>55</v>
       </c>
@@ -3111,7 +3117,7 @@
       <c r="K86" s="5"/>
       <c r="L86" s="5"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A87" s="11" t="s">
         <v>57</v>
       </c>
@@ -3132,7 +3138,7 @@
       <c r="K87" s="5"/>
       <c r="L87" s="5"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A88" s="8"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3149,7 +3155,7 @@
       <c r="K88" s="5"/>
       <c r="L88" s="5"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A89" s="8"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -3166,7 +3172,7 @@
       <c r="K89" s="5"/>
       <c r="L89" s="5"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A90" s="9" t="s">
         <v>30</v>
       </c>
@@ -3190,7 +3196,7 @@
       <c r="K90" s="6"/>
       <c r="L90" s="5"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A91" s="11" t="s">
         <v>17</v>
       </c>
@@ -3212,7 +3218,7 @@
       <c r="K91" s="6"/>
       <c r="L91" s="5"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A92" s="10" t="s">
         <v>28</v>
       </c>
@@ -3234,7 +3240,7 @@
       <c r="K92" s="6"/>
       <c r="L92" s="5"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A93" s="11"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
@@ -3248,7 +3254,7 @@
       <c r="K93" s="6"/>
       <c r="L93" s="5"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A94" s="11"/>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
@@ -3262,78 +3268,78 @@
       <c r="K94" s="5"/>
       <c r="L94" s="5"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A95" s="14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A96" s="12"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A97" s="12"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A98" s="12"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A99" s="12"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A100" s="12"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A101" s="12"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A102" s="12"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A103" s="12"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A104" s="12"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A105" s="12"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A106" s="12"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A107" s="12"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A108" s="12"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A109" s="12"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A110" s="12"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A111" s="12"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A112" s="12"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A113" s="12"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A114" s="12"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A115" s="12"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A116" s="12"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A117" s="12"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A118" s="13"/>
     </row>
   </sheetData>
@@ -3359,7 +3365,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3429,7 +3435,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3447,7 +3453,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Second Scene Basic, and multithreading, multiTexture
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A410E01-9FDB-44A1-99CB-9624548FF502}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD9CAAF-1BBE-4794-A0BC-2A8F9228B121}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="118">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -396,6 +396,10 @@
   </si>
   <si>
     <t>III</t>
+  </si>
+  <si>
+    <t>III</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1000,16 +1004,16 @@
       <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="106.44140625" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="1" max="1" width="106.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="7" width="25.44140625" customWidth="1"/>
-    <col min="8" max="9" width="25.88671875" customWidth="1"/>
-    <col min="10" max="11" width="24.44140625" customWidth="1"/>
-    <col min="12" max="12" width="24.109375" customWidth="1"/>
-    <col min="13" max="14" width="9.109375" customWidth="1"/>
+    <col min="4" max="7" width="25.42578125" customWidth="1"/>
+    <col min="8" max="9" width="25.85546875" customWidth="1"/>
+    <col min="10" max="11" width="24.42578125" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1624,9 +1628,7 @@
       <c r="D22" s="5">
         <v>2</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>116</v>
-      </c>
+      <c r="E22" s="2"/>
       <c r="F22" s="3"/>
       <c r="G22" s="16">
         <f t="shared" si="0"/>
@@ -2002,7 +2004,9 @@
       <c r="D38" s="5">
         <v>1</v>
       </c>
-      <c r="E38" s="2"/>
+      <c r="E38" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="F38" s="3"/>
       <c r="G38" s="16">
         <f t="shared" si="0"/>
@@ -2505,7 +2509,9 @@
       <c r="D59" s="5">
         <v>4</v>
       </c>
-      <c r="E59" s="2"/>
+      <c r="E59" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="F59" s="3"/>
       <c r="G59" s="16">
         <f t="shared" si="0"/>
@@ -3095,7 +3101,9 @@
       <c r="D85" s="5">
         <v>5</v>
       </c>
-      <c r="E85" s="2"/>
+      <c r="E85" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="F85" s="3"/>
       <c r="G85" s="16">
         <f t="shared" si="1"/>
@@ -3376,7 +3384,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3446,7 +3454,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3464,7 +3472,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
CommandList unfinished, Drawinstance is kind of buggy
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EEB4050-183C-4F05-AE43-5AAEF96D04A4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C0C1C7-F9CA-42A2-9C87-691865D9EF51}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="118">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -363,6 +363,10 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
+    <t>X</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
     <t>II</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -371,7 +375,7 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>II</t>
+    <t>Demonstrate modified vertex grid based on input map or sine wave in vertex shader. (ex: Waving Flag, Heightmap Terrain)</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
@@ -379,18 +383,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>Demonstrate modified vertex grid based on input map or sine wave in vertex shader. (ex: Waving Flag, Heightmap Terrain)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>II</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>X</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>III</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -398,11 +390,13 @@
     <t>III</t>
   </si>
   <si>
-    <t>III</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>space Skybox -- Created by 'amethyst7' aka Chris Matz. WEB site: http://amethyst7.gotdoofed.com</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +998,7 @@
   <dimension ref="A1:L118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85"/>
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1136,15 +1130,15 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1213,16 +1207,16 @@
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 20,0)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J6" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) - 20,0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="15">
         <f>IF(L4 &gt; 60, SUM(-60,L4),0)</f>
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1358,15 +1352,15 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1460,10 +1454,10 @@
         <v>4</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G14" s="16">
         <f t="shared" si="0"/>
@@ -1489,10 +1483,10 @@
         <v>2</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="G15" s="16">
         <f t="shared" si="0"/>
@@ -1635,11 +1629,15 @@
       <c r="D22" s="5">
         <v>2</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="3"/>
+      <c r="E22" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="G22" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
@@ -2011,9 +2009,7 @@
       <c r="D38" s="5">
         <v>1</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>116</v>
-      </c>
+      <c r="E38" s="2"/>
       <c r="F38" s="3"/>
       <c r="G38" s="16">
         <f t="shared" si="0"/>
@@ -2067,7 +2063,9 @@
       <c r="D40" s="5">
         <v>3</v>
       </c>
-      <c r="E40" s="2"/>
+      <c r="E40" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="F40" s="3"/>
       <c r="G40" s="16">
         <f t="shared" si="0"/>
@@ -2206,7 +2204,7 @@
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B46" s="1">
         <v>3</v>
@@ -2221,7 +2219,7 @@
         <v>104</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G46" s="16">
         <f t="shared" si="0"/>
@@ -2461,10 +2459,10 @@
         <v>2</v>
       </c>
       <c r="E57" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="G57" s="16">
         <f t="shared" si="0"/>
@@ -2490,10 +2488,10 @@
         <v>3</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G58" s="16">
         <f t="shared" si="0"/>
@@ -2519,7 +2517,7 @@
         <v>4</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F59" s="3"/>
       <c r="G59" s="16">
@@ -2599,10 +2597,10 @@
         <v>2</v>
       </c>
       <c r="E63" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F63" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="G63" s="16">
         <f t="shared" si="0"/>
@@ -2657,10 +2655,10 @@
         <v>1</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G65" s="16">
         <f t="shared" si="0"/>
@@ -2715,10 +2713,10 @@
         <v>4</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G67" s="16">
         <f t="shared" si="0"/>
@@ -3088,10 +3086,10 @@
         <v>4</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G84" s="16">
         <f t="shared" si="1"/>
@@ -3113,12 +3111,14 @@
         <v>5</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F85" s="3"/>
+        <v>114</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="G85" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H85" s="5"/>
       <c r="I85" s="5"/>
@@ -3240,7 +3240,7 @@
         <v>106</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
@@ -3264,7 +3264,7 @@
         <v>106</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
@@ -3308,7 +3308,9 @@
       </c>
     </row>
     <row r="96" spans="1:12">
-      <c r="A96" s="12"/>
+      <c r="A96" s="12" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="12"/>
@@ -3399,7 +3401,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
DrawInstance Done, fixed look at feature(kind of)
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C0C1C7-F9CA-42A2-9C87-691865D9EF51}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A2D15A-9D60-4E24-888E-8417BF99CFD7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -997,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1134,11 +1134,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1211,12 +1211,12 @@
       </c>
       <c r="J6" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) - 20,0)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="15">
         <f>IF(L4 &gt; 60, SUM(-60,L4),0)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1352,15 +1352,15 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -2066,10 +2066,12 @@
       <c r="E40" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F40" s="3"/>
+      <c r="F40" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="G40" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -2516,9 +2518,7 @@
       <c r="D59" s="5">
         <v>4</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>114</v>
-      </c>
+      <c r="E59" s="2"/>
       <c r="F59" s="3"/>
       <c r="G59" s="16">
         <f t="shared" si="0"/>
@@ -3401,7 +3401,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>